<commit_message>
count of checkStyle errors on 6th July 09(Mon)
SVN-Revision: 22254
</commit_message>
<xml_diff>
--- a/Documents/Build++/Build++ Assignments.xlsx
+++ b/Documents/Build++/Build++ Assignments.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="18975" windowHeight="8385"/>
+    <workbookView xWindow="120" yWindow="120" windowWidth="15480" windowHeight="8385"/>
   </bookViews>
   <sheets>
     <sheet name="CheckStyle &amp; SpellChecker" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="114210"/>
 </workbook>
 </file>
 
@@ -240,10 +240,9 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -255,13 +254,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor indexed="13"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79998168889431442"/>
+        <fgColor indexed="27"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -281,9 +280,7 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -296,7 +293,9 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -315,20 +314,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -628,8 +627,8 @@
   <dimension ref="A1:M54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -640,68 +639,68 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="1" customFormat="1" ht="30">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9" t="s">
+      <c r="E1" s="8"/>
+      <c r="F1" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9" t="s">
+      <c r="G1" s="8"/>
+      <c r="H1" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9" t="s">
+      <c r="I1" s="8"/>
+      <c r="J1" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9" t="s">
+      <c r="K1" s="8"/>
+      <c r="L1" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="M1" s="9"/>
+      <c r="M1" s="8"/>
     </row>
     <row r="2" spans="1:13">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="7" t="s">
+      <c r="A2" s="4"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="I2" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="J2" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="K2" s="7" t="s">
+      <c r="K2" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="L2" s="7" t="s">
+      <c r="L2" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="M2" s="7" t="s">
+      <c r="M2" s="6" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1119,7 +1118,7 @@
       </c>
       <c r="C48" s="3"/>
     </row>
-    <row r="49" spans="1:3" ht="30">
+    <row r="49" spans="1:4" ht="30">
       <c r="A49" s="3" t="s">
         <v>0</v>
       </c>
@@ -1128,7 +1127,7 @@
       </c>
       <c r="C49" s="3"/>
     </row>
-    <row r="50" spans="1:3" ht="30">
+    <row r="50" spans="1:4" ht="30">
       <c r="A50" s="3" t="s">
         <v>1</v>
       </c>
@@ -1136,8 +1135,11 @@
         <v>52</v>
       </c>
       <c r="C50" s="3"/>
-    </row>
-    <row r="51" spans="1:3" ht="30">
+      <c r="D50">
+        <v>7862</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="30">
       <c r="A51" s="3" t="s">
         <v>27</v>
       </c>
@@ -1145,8 +1147,11 @@
         <v>52</v>
       </c>
       <c r="C51" s="3"/>
-    </row>
-    <row r="52" spans="1:3" ht="30">
+      <c r="D51">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="30">
       <c r="A52" s="3" t="s">
         <v>28</v>
       </c>
@@ -1154,8 +1159,11 @@
         <v>52</v>
       </c>
       <c r="C52" s="3"/>
-    </row>
-    <row r="53" spans="1:3" ht="45">
+      <c r="D52">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="45">
       <c r="A53" s="3" t="s">
         <v>29</v>
       </c>
@@ -1163,8 +1171,11 @@
         <v>52</v>
       </c>
       <c r="C53" s="3"/>
-    </row>
-    <row r="54" spans="1:3" ht="30">
+      <c r="D53">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="30">
       <c r="A54" s="3" t="s">
         <v>30</v>
       </c>
@@ -1172,18 +1183,19 @@
         <v>52</v>
       </c>
       <c r="C54" s="3"/>
+      <c r="D54">
+        <v>1812</v>
+      </c>
     </row>
   </sheetData>
-  <sortState ref="A1:B1048576">
-    <sortCondition ref="B1"/>
-  </sortState>
   <mergeCells count="5">
+    <mergeCell ref="L1:M1"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="H1:I1"/>
     <mergeCell ref="J1:K1"/>
-    <mergeCell ref="L1:M1"/>
   </mergeCells>
+  <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
@@ -1213,26 +1225,26 @@
       <c r="C1" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4" t="s">
+      <c r="E1" s="9"/>
+      <c r="F1" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4" t="s">
+      <c r="G1" s="9"/>
+      <c r="H1" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4" t="s">
+      <c r="I1" s="9"/>
+      <c r="J1" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4" t="s">
+      <c r="K1" s="9"/>
+      <c r="L1" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="M1" s="4"/>
+      <c r="M1" s="9"/>
     </row>
     <row r="2" spans="1:13">
       <c r="A2" s="2"/>
@@ -1269,7 +1281,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="165">
+    <row r="3" spans="1:13" ht="45">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -1278,7 +1290,7 @@
       </c>
       <c r="C3" s="3"/>
     </row>
-    <row r="4" spans="1:13" ht="180">
+    <row r="4" spans="1:13" ht="45">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -1287,7 +1299,7 @@
       </c>
       <c r="C4" s="3"/>
     </row>
-    <row r="5" spans="1:13" ht="180">
+    <row r="5" spans="1:13" ht="45">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
@@ -1296,7 +1308,7 @@
       </c>
       <c r="C5" s="3"/>
     </row>
-    <row r="6" spans="1:13" ht="180">
+    <row r="6" spans="1:13" ht="45">
       <c r="A6" s="3" t="s">
         <v>6</v>
       </c>
@@ -1305,7 +1317,7 @@
       </c>
       <c r="C6" s="3"/>
     </row>
-    <row r="7" spans="1:13" ht="165">
+    <row r="7" spans="1:13" ht="30">
       <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
@@ -1314,7 +1326,7 @@
       </c>
       <c r="C7" s="3"/>
     </row>
-    <row r="8" spans="1:13" ht="165">
+    <row r="8" spans="1:13" ht="30">
       <c r="A8" s="3" t="s">
         <v>8</v>
       </c>
@@ -1323,7 +1335,7 @@
       </c>
       <c r="C8" s="3"/>
     </row>
-    <row r="9" spans="1:13" ht="180">
+    <row r="9" spans="1:13" ht="45">
       <c r="A9" s="3" t="s">
         <v>17</v>
       </c>
@@ -1332,7 +1344,7 @@
       </c>
       <c r="C9" s="3"/>
     </row>
-    <row r="10" spans="1:13" ht="180">
+    <row r="10" spans="1:13" ht="45">
       <c r="A10" s="3" t="s">
         <v>18</v>
       </c>
@@ -1341,7 +1353,7 @@
       </c>
       <c r="C10" s="3"/>
     </row>
-    <row r="11" spans="1:13" ht="180">
+    <row r="11" spans="1:13" ht="45">
       <c r="A11" s="3" t="s">
         <v>32</v>
       </c>
@@ -1350,7 +1362,7 @@
       </c>
       <c r="C11" s="3"/>
     </row>
-    <row r="12" spans="1:13" ht="180">
+    <row r="12" spans="1:13" ht="45">
       <c r="A12" s="3" t="s">
         <v>50</v>
       </c>
@@ -1359,7 +1371,7 @@
       </c>
       <c r="C12" s="3"/>
     </row>
-    <row r="13" spans="1:13" ht="150">
+    <row r="13" spans="1:13" ht="30">
       <c r="A13" s="3" t="s">
         <v>16</v>
       </c>
@@ -1368,7 +1380,7 @@
       </c>
       <c r="C13" s="3"/>
     </row>
-    <row r="14" spans="1:13" ht="165">
+    <row r="14" spans="1:13" ht="30">
       <c r="A14" s="3" t="s">
         <v>37</v>
       </c>
@@ -1377,7 +1389,7 @@
       </c>
       <c r="C14" s="3"/>
     </row>
-    <row r="15" spans="1:13" ht="180">
+    <row r="15" spans="1:13" ht="45">
       <c r="A15" s="3" t="s">
         <v>38</v>
       </c>
@@ -1386,7 +1398,7 @@
       </c>
       <c r="C15" s="3"/>
     </row>
-    <row r="16" spans="1:13" ht="165">
+    <row r="16" spans="1:13" ht="30">
       <c r="A16" s="3" t="s">
         <v>39</v>
       </c>
@@ -1395,7 +1407,7 @@
       </c>
       <c r="C16" s="3"/>
     </row>
-    <row r="17" spans="1:3" ht="165">
+    <row r="17" spans="1:3" ht="30">
       <c r="A17" s="3" t="s">
         <v>40</v>
       </c>
@@ -1404,7 +1416,7 @@
       </c>
       <c r="C17" s="3"/>
     </row>
-    <row r="18" spans="1:3" ht="165">
+    <row r="18" spans="1:3" ht="45">
       <c r="A18" s="3" t="s">
         <v>41</v>
       </c>
@@ -1413,7 +1425,7 @@
       </c>
       <c r="C18" s="3"/>
     </row>
-    <row r="19" spans="1:3" ht="150">
+    <row r="19" spans="1:3" ht="30">
       <c r="A19" s="3" t="s">
         <v>42</v>
       </c>
@@ -1422,7 +1434,7 @@
       </c>
       <c r="C19" s="3"/>
     </row>
-    <row r="20" spans="1:3" ht="180">
+    <row r="20" spans="1:3" ht="45">
       <c r="A20" s="3" t="s">
         <v>43</v>
       </c>
@@ -1431,7 +1443,7 @@
       </c>
       <c r="C20" s="3"/>
     </row>
-    <row r="21" spans="1:3" ht="165">
+    <row r="21" spans="1:3" ht="30">
       <c r="A21" s="3" t="s">
         <v>44</v>
       </c>
@@ -1440,7 +1452,7 @@
       </c>
       <c r="C21" s="3"/>
     </row>
-    <row r="22" spans="1:3" ht="150">
+    <row r="22" spans="1:3" ht="30">
       <c r="A22" s="3" t="s">
         <v>5</v>
       </c>
@@ -1449,7 +1461,7 @@
       </c>
       <c r="C22" s="3"/>
     </row>
-    <row r="23" spans="1:3" ht="150">
+    <row r="23" spans="1:3" ht="30">
       <c r="A23" s="3" t="s">
         <v>22</v>
       </c>
@@ -1458,7 +1470,7 @@
       </c>
       <c r="C23" s="3"/>
     </row>
-    <row r="24" spans="1:3" ht="165">
+    <row r="24" spans="1:3" ht="30">
       <c r="A24" s="3" t="s">
         <v>23</v>
       </c>
@@ -1467,7 +1479,7 @@
       </c>
       <c r="C24" s="3"/>
     </row>
-    <row r="25" spans="1:3" ht="195">
+    <row r="25" spans="1:3" ht="45">
       <c r="A25" s="3" t="s">
         <v>24</v>
       </c>
@@ -1476,7 +1488,7 @@
       </c>
       <c r="C25" s="3"/>
     </row>
-    <row r="26" spans="1:3" ht="180">
+    <row r="26" spans="1:3" ht="45">
       <c r="A26" s="3" t="s">
         <v>25</v>
       </c>
@@ -1485,7 +1497,7 @@
       </c>
       <c r="C26" s="3"/>
     </row>
-    <row r="27" spans="1:3" ht="165">
+    <row r="27" spans="1:3" ht="45">
       <c r="A27" s="3" t="s">
         <v>26</v>
       </c>
@@ -1494,7 +1506,7 @@
       </c>
       <c r="C27" s="3"/>
     </row>
-    <row r="28" spans="1:3" ht="150">
+    <row r="28" spans="1:3" ht="30">
       <c r="A28" s="3" t="s">
         <v>45</v>
       </c>
@@ -1503,7 +1515,7 @@
       </c>
       <c r="C28" s="3"/>
     </row>
-    <row r="29" spans="1:3" ht="150">
+    <row r="29" spans="1:3" ht="30">
       <c r="A29" s="3" t="s">
         <v>9</v>
       </c>
@@ -1512,7 +1524,7 @@
       </c>
       <c r="C29" s="3"/>
     </row>
-    <row r="30" spans="1:3" ht="165">
+    <row r="30" spans="1:3" ht="45">
       <c r="A30" s="3" t="s">
         <v>10</v>
       </c>
@@ -1521,7 +1533,7 @@
       </c>
       <c r="C30" s="3"/>
     </row>
-    <row r="31" spans="1:3" ht="165">
+    <row r="31" spans="1:3" ht="30">
       <c r="A31" s="3" t="s">
         <v>11</v>
       </c>
@@ -1530,7 +1542,7 @@
       </c>
       <c r="C31" s="3"/>
     </row>
-    <row r="32" spans="1:3" ht="150">
+    <row r="32" spans="1:3" ht="30">
       <c r="A32" s="3" t="s">
         <v>19</v>
       </c>
@@ -1539,7 +1551,7 @@
       </c>
       <c r="C32" s="3"/>
     </row>
-    <row r="33" spans="1:3" ht="150">
+    <row r="33" spans="1:3" ht="30">
       <c r="A33" s="3" t="s">
         <v>20</v>
       </c>
@@ -1548,7 +1560,7 @@
       </c>
       <c r="C33" s="3"/>
     </row>
-    <row r="34" spans="1:3" ht="165">
+    <row r="34" spans="1:3" ht="45">
       <c r="A34" s="3" t="s">
         <v>31</v>
       </c>
@@ -1557,7 +1569,7 @@
       </c>
       <c r="C34" s="3"/>
     </row>
-    <row r="35" spans="1:3" ht="150">
+    <row r="35" spans="1:3" ht="30">
       <c r="A35" s="3" t="s">
         <v>33</v>
       </c>
@@ -1566,7 +1578,7 @@
       </c>
       <c r="C35" s="3"/>
     </row>
-    <row r="36" spans="1:3" ht="150">
+    <row r="36" spans="1:3" ht="30">
       <c r="A36" s="3" t="s">
         <v>34</v>
       </c>
@@ -1575,7 +1587,7 @@
       </c>
       <c r="C36" s="3"/>
     </row>
-    <row r="37" spans="1:3" ht="150">
+    <row r="37" spans="1:3" ht="30">
       <c r="A37" s="3" t="s">
         <v>35</v>
       </c>
@@ -1584,7 +1596,7 @@
       </c>
       <c r="C37" s="3"/>
     </row>
-    <row r="38" spans="1:3" ht="150">
+    <row r="38" spans="1:3" ht="30">
       <c r="A38" s="3" t="s">
         <v>36</v>
       </c>
@@ -1593,7 +1605,7 @@
       </c>
       <c r="C38" s="3"/>
     </row>
-    <row r="39" spans="1:3" ht="150">
+    <row r="39" spans="1:3" ht="30">
       <c r="A39" s="3" t="s">
         <v>46</v>
       </c>
@@ -1602,7 +1614,7 @@
       </c>
       <c r="C39" s="3"/>
     </row>
-    <row r="40" spans="1:3" ht="150">
+    <row r="40" spans="1:3" ht="30">
       <c r="A40" s="3" t="s">
         <v>47</v>
       </c>
@@ -1611,7 +1623,7 @@
       </c>
       <c r="C40" s="3"/>
     </row>
-    <row r="41" spans="1:3" ht="150">
+    <row r="41" spans="1:3" ht="30">
       <c r="A41" s="3" t="s">
         <v>48</v>
       </c>
@@ -1620,7 +1632,7 @@
       </c>
       <c r="C41" s="3"/>
     </row>
-    <row r="42" spans="1:3" ht="165">
+    <row r="42" spans="1:3" ht="30">
       <c r="A42" s="3" t="s">
         <v>49</v>
       </c>
@@ -1629,7 +1641,7 @@
       </c>
       <c r="C42" s="3"/>
     </row>
-    <row r="43" spans="1:3" ht="165">
+    <row r="43" spans="1:3" ht="30">
       <c r="A43" s="3" t="s">
         <v>12</v>
       </c>
@@ -1638,7 +1650,7 @@
       </c>
       <c r="C43" s="3"/>
     </row>
-    <row r="44" spans="1:3" ht="150">
+    <row r="44" spans="1:3" ht="30">
       <c r="A44" s="3" t="s">
         <v>13</v>
       </c>
@@ -1647,7 +1659,7 @@
       </c>
       <c r="C44" s="3"/>
     </row>
-    <row r="45" spans="1:3" ht="150">
+    <row r="45" spans="1:3" ht="30">
       <c r="A45" s="3" t="s">
         <v>14</v>
       </c>
@@ -1656,7 +1668,7 @@
       </c>
       <c r="C45" s="3"/>
     </row>
-    <row r="46" spans="1:3" ht="150">
+    <row r="46" spans="1:3" ht="30">
       <c r="A46" s="3" t="s">
         <v>15</v>
       </c>
@@ -1665,7 +1677,7 @@
       </c>
       <c r="C46" s="3"/>
     </row>
-    <row r="47" spans="1:3" ht="165">
+    <row r="47" spans="1:3" ht="30">
       <c r="A47" s="3" t="s">
         <v>21</v>
       </c>
@@ -1674,7 +1686,7 @@
       </c>
       <c r="C47" s="3"/>
     </row>
-    <row r="48" spans="1:3" ht="135">
+    <row r="48" spans="1:3" ht="30">
       <c r="A48" s="3" t="s">
         <v>51</v>
       </c>
@@ -1683,7 +1695,7 @@
       </c>
       <c r="C48" s="3"/>
     </row>
-    <row r="49" spans="1:3" ht="105">
+    <row r="49" spans="1:3" ht="30">
       <c r="A49" s="3" t="s">
         <v>0</v>
       </c>
@@ -1692,7 +1704,7 @@
       </c>
       <c r="C49" s="3"/>
     </row>
-    <row r="50" spans="1:3" ht="150">
+    <row r="50" spans="1:3" ht="30">
       <c r="A50" s="3" t="s">
         <v>1</v>
       </c>
@@ -1701,7 +1713,7 @@
       </c>
       <c r="C50" s="3"/>
     </row>
-    <row r="51" spans="1:3" ht="165">
+    <row r="51" spans="1:3" ht="30">
       <c r="A51" s="3" t="s">
         <v>27</v>
       </c>
@@ -1710,7 +1722,7 @@
       </c>
       <c r="C51" s="3"/>
     </row>
-    <row r="52" spans="1:3" ht="165">
+    <row r="52" spans="1:3" ht="30">
       <c r="A52" s="3" t="s">
         <v>28</v>
       </c>
@@ -1719,7 +1731,7 @@
       </c>
       <c r="C52" s="3"/>
     </row>
-    <row r="53" spans="1:3" ht="195">
+    <row r="53" spans="1:3" ht="45">
       <c r="A53" s="3" t="s">
         <v>29</v>
       </c>
@@ -1728,7 +1740,7 @@
       </c>
       <c r="C53" s="3"/>
     </row>
-    <row r="54" spans="1:3" ht="150">
+    <row r="54" spans="1:3" ht="30">
       <c r="A54" s="3" t="s">
         <v>30</v>
       </c>
@@ -1739,12 +1751,13 @@
     </row>
   </sheetData>
   <mergeCells count="5">
+    <mergeCell ref="L1:M1"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="H1:I1"/>
     <mergeCell ref="J1:K1"/>
-    <mergeCell ref="L1:M1"/>
   </mergeCells>
+  <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1774,26 +1787,26 @@
       <c r="C1" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4" t="s">
+      <c r="E1" s="9"/>
+      <c r="F1" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4" t="s">
+      <c r="G1" s="9"/>
+      <c r="H1" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4" t="s">
+      <c r="I1" s="9"/>
+      <c r="J1" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4" t="s">
+      <c r="K1" s="9"/>
+      <c r="L1" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="M1" s="4"/>
+      <c r="M1" s="9"/>
     </row>
     <row r="2" spans="1:13">
       <c r="A2" s="2"/>
@@ -1830,7 +1843,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="165">
+    <row r="3" spans="1:13" ht="45">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -1839,7 +1852,7 @@
       </c>
       <c r="C3" s="3"/>
     </row>
-    <row r="4" spans="1:13" ht="180">
+    <row r="4" spans="1:13" ht="45">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -1848,7 +1861,7 @@
       </c>
       <c r="C4" s="3"/>
     </row>
-    <row r="5" spans="1:13" ht="180">
+    <row r="5" spans="1:13" ht="45">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
@@ -1857,7 +1870,7 @@
       </c>
       <c r="C5" s="3"/>
     </row>
-    <row r="6" spans="1:13" ht="180">
+    <row r="6" spans="1:13" ht="45">
       <c r="A6" s="3" t="s">
         <v>6</v>
       </c>
@@ -1866,7 +1879,7 @@
       </c>
       <c r="C6" s="3"/>
     </row>
-    <row r="7" spans="1:13" ht="165">
+    <row r="7" spans="1:13" ht="45">
       <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
@@ -1875,7 +1888,7 @@
       </c>
       <c r="C7" s="3"/>
     </row>
-    <row r="8" spans="1:13" ht="165">
+    <row r="8" spans="1:13" ht="45">
       <c r="A8" s="3" t="s">
         <v>8</v>
       </c>
@@ -1884,7 +1897,7 @@
       </c>
       <c r="C8" s="3"/>
     </row>
-    <row r="9" spans="1:13" ht="180">
+    <row r="9" spans="1:13" ht="45">
       <c r="A9" s="3" t="s">
         <v>17</v>
       </c>
@@ -1893,7 +1906,7 @@
       </c>
       <c r="C9" s="3"/>
     </row>
-    <row r="10" spans="1:13" ht="180">
+    <row r="10" spans="1:13" ht="45">
       <c r="A10" s="3" t="s">
         <v>18</v>
       </c>
@@ -1902,7 +1915,7 @@
       </c>
       <c r="C10" s="3"/>
     </row>
-    <row r="11" spans="1:13" ht="180">
+    <row r="11" spans="1:13" ht="45">
       <c r="A11" s="3" t="s">
         <v>32</v>
       </c>
@@ -1911,7 +1924,7 @@
       </c>
       <c r="C11" s="3"/>
     </row>
-    <row r="12" spans="1:13" ht="180">
+    <row r="12" spans="1:13" ht="45">
       <c r="A12" s="3" t="s">
         <v>50</v>
       </c>
@@ -1920,7 +1933,7 @@
       </c>
       <c r="C12" s="3"/>
     </row>
-    <row r="13" spans="1:13" ht="150">
+    <row r="13" spans="1:13" ht="30">
       <c r="A13" s="3" t="s">
         <v>16</v>
       </c>
@@ -1929,7 +1942,7 @@
       </c>
       <c r="C13" s="3"/>
     </row>
-    <row r="14" spans="1:13" ht="165">
+    <row r="14" spans="1:13" ht="45">
       <c r="A14" s="3" t="s">
         <v>37</v>
       </c>
@@ -1938,7 +1951,7 @@
       </c>
       <c r="C14" s="3"/>
     </row>
-    <row r="15" spans="1:13" ht="180">
+    <row r="15" spans="1:13" ht="45">
       <c r="A15" s="3" t="s">
         <v>38</v>
       </c>
@@ -1947,7 +1960,7 @@
       </c>
       <c r="C15" s="3"/>
     </row>
-    <row r="16" spans="1:13" ht="165">
+    <row r="16" spans="1:13" ht="45">
       <c r="A16" s="3" t="s">
         <v>39</v>
       </c>
@@ -1956,7 +1969,7 @@
       </c>
       <c r="C16" s="3"/>
     </row>
-    <row r="17" spans="1:3" ht="165">
+    <row r="17" spans="1:3" ht="45">
       <c r="A17" s="3" t="s">
         <v>40</v>
       </c>
@@ -1965,7 +1978,7 @@
       </c>
       <c r="C17" s="3"/>
     </row>
-    <row r="18" spans="1:3" ht="165">
+    <row r="18" spans="1:3" ht="45">
       <c r="A18" s="3" t="s">
         <v>41</v>
       </c>
@@ -1974,7 +1987,7 @@
       </c>
       <c r="C18" s="3"/>
     </row>
-    <row r="19" spans="1:3" ht="150">
+    <row r="19" spans="1:3" ht="45">
       <c r="A19" s="3" t="s">
         <v>42</v>
       </c>
@@ -1983,7 +1996,7 @@
       </c>
       <c r="C19" s="3"/>
     </row>
-    <row r="20" spans="1:3" ht="180">
+    <row r="20" spans="1:3" ht="45">
       <c r="A20" s="3" t="s">
         <v>43</v>
       </c>
@@ -1992,7 +2005,7 @@
       </c>
       <c r="C20" s="3"/>
     </row>
-    <row r="21" spans="1:3" ht="165">
+    <row r="21" spans="1:3" ht="45">
       <c r="A21" s="3" t="s">
         <v>44</v>
       </c>
@@ -2001,7 +2014,7 @@
       </c>
       <c r="C21" s="3"/>
     </row>
-    <row r="22" spans="1:3" ht="150">
+    <row r="22" spans="1:3" ht="45">
       <c r="A22" s="3" t="s">
         <v>5</v>
       </c>
@@ -2010,7 +2023,7 @@
       </c>
       <c r="C22" s="3"/>
     </row>
-    <row r="23" spans="1:3" ht="150">
+    <row r="23" spans="1:3" ht="30">
       <c r="A23" s="3" t="s">
         <v>22</v>
       </c>
@@ -2019,7 +2032,7 @@
       </c>
       <c r="C23" s="3"/>
     </row>
-    <row r="24" spans="1:3" ht="165">
+    <row r="24" spans="1:3" ht="45">
       <c r="A24" s="3" t="s">
         <v>23</v>
       </c>
@@ -2028,7 +2041,7 @@
       </c>
       <c r="C24" s="3"/>
     </row>
-    <row r="25" spans="1:3" ht="195">
+    <row r="25" spans="1:3" ht="45">
       <c r="A25" s="3" t="s">
         <v>24</v>
       </c>
@@ -2037,7 +2050,7 @@
       </c>
       <c r="C25" s="3"/>
     </row>
-    <row r="26" spans="1:3" ht="180">
+    <row r="26" spans="1:3" ht="45">
       <c r="A26" s="3" t="s">
         <v>25</v>
       </c>
@@ -2046,7 +2059,7 @@
       </c>
       <c r="C26" s="3"/>
     </row>
-    <row r="27" spans="1:3" ht="165">
+    <row r="27" spans="1:3" ht="45">
       <c r="A27" s="3" t="s">
         <v>26</v>
       </c>
@@ -2055,7 +2068,7 @@
       </c>
       <c r="C27" s="3"/>
     </row>
-    <row r="28" spans="1:3" ht="150">
+    <row r="28" spans="1:3" ht="30">
       <c r="A28" s="3" t="s">
         <v>45</v>
       </c>
@@ -2064,7 +2077,7 @@
       </c>
       <c r="C28" s="3"/>
     </row>
-    <row r="29" spans="1:3" ht="150">
+    <row r="29" spans="1:3" ht="30">
       <c r="A29" s="3" t="s">
         <v>9</v>
       </c>
@@ -2073,7 +2086,7 @@
       </c>
       <c r="C29" s="3"/>
     </row>
-    <row r="30" spans="1:3" ht="165">
+    <row r="30" spans="1:3" ht="45">
       <c r="A30" s="3" t="s">
         <v>10</v>
       </c>
@@ -2082,7 +2095,7 @@
       </c>
       <c r="C30" s="3"/>
     </row>
-    <row r="31" spans="1:3" ht="165">
+    <row r="31" spans="1:3" ht="45">
       <c r="A31" s="3" t="s">
         <v>11</v>
       </c>
@@ -2091,7 +2104,7 @@
       </c>
       <c r="C31" s="3"/>
     </row>
-    <row r="32" spans="1:3" ht="150">
+    <row r="32" spans="1:3" ht="30">
       <c r="A32" s="3" t="s">
         <v>19</v>
       </c>
@@ -2100,7 +2113,7 @@
       </c>
       <c r="C32" s="3"/>
     </row>
-    <row r="33" spans="1:3" ht="150">
+    <row r="33" spans="1:3" ht="45">
       <c r="A33" s="3" t="s">
         <v>20</v>
       </c>
@@ -2109,7 +2122,7 @@
       </c>
       <c r="C33" s="3"/>
     </row>
-    <row r="34" spans="1:3" ht="165">
+    <row r="34" spans="1:3" ht="45">
       <c r="A34" s="3" t="s">
         <v>31</v>
       </c>
@@ -2118,7 +2131,7 @@
       </c>
       <c r="C34" s="3"/>
     </row>
-    <row r="35" spans="1:3" ht="150">
+    <row r="35" spans="1:3" ht="30">
       <c r="A35" s="3" t="s">
         <v>33</v>
       </c>
@@ -2127,7 +2140,7 @@
       </c>
       <c r="C35" s="3"/>
     </row>
-    <row r="36" spans="1:3" ht="150">
+    <row r="36" spans="1:3" ht="45">
       <c r="A36" s="3" t="s">
         <v>34</v>
       </c>
@@ -2136,7 +2149,7 @@
       </c>
       <c r="C36" s="3"/>
     </row>
-    <row r="37" spans="1:3" ht="150">
+    <row r="37" spans="1:3" ht="30">
       <c r="A37" s="3" t="s">
         <v>35</v>
       </c>
@@ -2145,7 +2158,7 @@
       </c>
       <c r="C37" s="3"/>
     </row>
-    <row r="38" spans="1:3" ht="150">
+    <row r="38" spans="1:3" ht="30">
       <c r="A38" s="3" t="s">
         <v>36</v>
       </c>
@@ -2154,7 +2167,7 @@
       </c>
       <c r="C38" s="3"/>
     </row>
-    <row r="39" spans="1:3" ht="150">
+    <row r="39" spans="1:3" ht="30">
       <c r="A39" s="3" t="s">
         <v>46</v>
       </c>
@@ -2163,7 +2176,7 @@
       </c>
       <c r="C39" s="3"/>
     </row>
-    <row r="40" spans="1:3" ht="150">
+    <row r="40" spans="1:3" ht="30">
       <c r="A40" s="3" t="s">
         <v>47</v>
       </c>
@@ -2172,7 +2185,7 @@
       </c>
       <c r="C40" s="3"/>
     </row>
-    <row r="41" spans="1:3" ht="150">
+    <row r="41" spans="1:3" ht="45">
       <c r="A41" s="3" t="s">
         <v>48</v>
       </c>
@@ -2181,7 +2194,7 @@
       </c>
       <c r="C41" s="3"/>
     </row>
-    <row r="42" spans="1:3" ht="165">
+    <row r="42" spans="1:3" ht="45">
       <c r="A42" s="3" t="s">
         <v>49</v>
       </c>
@@ -2190,7 +2203,7 @@
       </c>
       <c r="C42" s="3"/>
     </row>
-    <row r="43" spans="1:3" ht="165">
+    <row r="43" spans="1:3" ht="45">
       <c r="A43" s="3" t="s">
         <v>12</v>
       </c>
@@ -2199,7 +2212,7 @@
       </c>
       <c r="C43" s="3"/>
     </row>
-    <row r="44" spans="1:3" ht="150">
+    <row r="44" spans="1:3" ht="30">
       <c r="A44" s="3" t="s">
         <v>13</v>
       </c>
@@ -2208,7 +2221,7 @@
       </c>
       <c r="C44" s="3"/>
     </row>
-    <row r="45" spans="1:3" ht="150">
+    <row r="45" spans="1:3" ht="45">
       <c r="A45" s="3" t="s">
         <v>14</v>
       </c>
@@ -2217,7 +2230,7 @@
       </c>
       <c r="C45" s="3"/>
     </row>
-    <row r="46" spans="1:3" ht="150">
+    <row r="46" spans="1:3" ht="30">
       <c r="A46" s="3" t="s">
         <v>15</v>
       </c>
@@ -2226,7 +2239,7 @@
       </c>
       <c r="C46" s="3"/>
     </row>
-    <row r="47" spans="1:3" ht="165">
+    <row r="47" spans="1:3" ht="45">
       <c r="A47" s="3" t="s">
         <v>21</v>
       </c>
@@ -2235,7 +2248,7 @@
       </c>
       <c r="C47" s="3"/>
     </row>
-    <row r="48" spans="1:3" ht="135">
+    <row r="48" spans="1:3" ht="30">
       <c r="A48" s="3" t="s">
         <v>51</v>
       </c>
@@ -2244,7 +2257,7 @@
       </c>
       <c r="C48" s="3"/>
     </row>
-    <row r="49" spans="1:3" ht="105">
+    <row r="49" spans="1:3" ht="30">
       <c r="A49" s="3" t="s">
         <v>0</v>
       </c>
@@ -2253,7 +2266,7 @@
       </c>
       <c r="C49" s="3"/>
     </row>
-    <row r="50" spans="1:3" ht="150">
+    <row r="50" spans="1:3" ht="30">
       <c r="A50" s="3" t="s">
         <v>1</v>
       </c>
@@ -2262,7 +2275,7 @@
       </c>
       <c r="C50" s="3"/>
     </row>
-    <row r="51" spans="1:3" ht="165">
+    <row r="51" spans="1:3" ht="45">
       <c r="A51" s="3" t="s">
         <v>27</v>
       </c>
@@ -2271,7 +2284,7 @@
       </c>
       <c r="C51" s="3"/>
     </row>
-    <row r="52" spans="1:3" ht="165">
+    <row r="52" spans="1:3" ht="45">
       <c r="A52" s="3" t="s">
         <v>28</v>
       </c>
@@ -2280,7 +2293,7 @@
       </c>
       <c r="C52" s="3"/>
     </row>
-    <row r="53" spans="1:3" ht="195">
+    <row r="53" spans="1:3" ht="45">
       <c r="A53" s="3" t="s">
         <v>29</v>
       </c>
@@ -2289,7 +2302,7 @@
       </c>
       <c r="C53" s="3"/>
     </row>
-    <row r="54" spans="1:3" ht="150">
+    <row r="54" spans="1:3" ht="30">
       <c r="A54" s="3" t="s">
         <v>30</v>
       </c>
@@ -2300,12 +2313,13 @@
     </row>
   </sheetData>
   <mergeCells count="5">
+    <mergeCell ref="L1:M1"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="H1:I1"/>
     <mergeCell ref="J1:K1"/>
-    <mergeCell ref="L1:M1"/>
   </mergeCells>
+  <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated count for only the check style warnings
SVN-Revision: 22271
</commit_message>
<xml_diff>
--- a/Documents/Build++/Build++ Assignments.xlsx
+++ b/Documents/Build++/Build++ Assignments.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="114210"/>
 </workbook>
 </file>
 
@@ -627,8 +627,8 @@
   <dimension ref="A1:M54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G16" sqref="G16"/>
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F47" sqref="F47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1146,7 +1146,7 @@
       </c>
       <c r="C48" s="3"/>
     </row>
-    <row r="49" spans="1:4" ht="30">
+    <row r="49" spans="1:5" ht="30">
       <c r="A49" s="3" t="s">
         <v>0</v>
       </c>
@@ -1155,7 +1155,7 @@
       </c>
       <c r="C49" s="3"/>
     </row>
-    <row r="50" spans="1:4" ht="30">
+    <row r="50" spans="1:5" ht="30">
       <c r="A50" s="3" t="s">
         <v>1</v>
       </c>
@@ -1164,10 +1164,13 @@
       </c>
       <c r="C50" s="3"/>
       <c r="D50">
-        <v>7862</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" ht="30">
+        <v>6873</v>
+      </c>
+      <c r="E50">
+        <v>5983</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="30">
       <c r="A51" s="3" t="s">
         <v>27</v>
       </c>
@@ -1179,7 +1182,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="30">
+    <row r="52" spans="1:5" ht="30">
       <c r="A52" s="3" t="s">
         <v>28</v>
       </c>
@@ -1191,7 +1194,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="45">
+    <row r="53" spans="1:5" ht="45">
       <c r="A53" s="3" t="s">
         <v>29</v>
       </c>
@@ -1203,7 +1206,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="30">
+    <row r="54" spans="1:5" ht="30">
       <c r="A54" s="3" t="s">
         <v>30</v>
       </c>

</xml_diff>